<commit_message>
Added initial agreements and summaries
</commit_message>
<xml_diff>
--- a/Comparison/regulatory_matrix.xlsx
+++ b/Comparison/regulatory_matrix.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mtmailmtsu-my.sharepoint.com/personal/aer7g_mtmail_mtsu_edu/Documents/DATA 6550/Project5/DATA6550_Privacy/Comparison/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_F25DC773A252ABDACC10484901D860A85ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BA2E679-B451-4CA7-81AA-F277D1C716BC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -18,8 +27,49 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Document Name</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>General Purpose</t>
+  </si>
+  <si>
+    <t>ProctorU Privacy Policy</t>
+  </si>
+  <si>
+    <t>ProctorU/Meazure Learning</t>
+  </si>
+  <si>
+    <t>Test taking software</t>
+  </si>
+  <si>
+    <t>Siemens Healthineers Privacy Notice</t>
+  </si>
+  <si>
+    <t>Siemens Healthineers</t>
+  </si>
+  <si>
+    <t>Website access</t>
+  </si>
+  <si>
+    <t>Vanderbilt Privacy Notice</t>
+  </si>
+  <si>
+    <t>Vanderbilt University Medical Center</t>
+  </si>
+  <si>
+    <t>Medical information</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,12 +79,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +105,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +387,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="39.21875" customWidth="1"/>
+    <col min="2" max="2" width="40.44140625" customWidth="1"/>
+    <col min="3" max="3" width="43.21875" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>